<commit_message>
add test data folder for neo4j aura
</commit_message>
<xml_diff>
--- a/ReadMe.xlsx
+++ b/ReadMe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xzhan50/projects/public-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E940B5D9-81D5-2244-B408-BBD78C2428EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FE4C1-2A58-C146-922C-CCD8741517E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="9220" windowWidth="28040" windowHeight="17440" xr2:uid="{8256766D-D95C-BC49-BB42-44E70E964C3B}"/>
+    <workbookView xWindow="6420" yWindow="2820" windowWidth="28040" windowHeight="17440" xr2:uid="{8256766D-D95C-BC49-BB42-44E70E964C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>file source</t>
   </si>
@@ -130,6 +130,24 @@
   </si>
   <si>
     <t>IEDB reference file of ALL loci ( unique records only)</t>
+  </si>
+  <si>
+    <t>used for hlR package, please DON'T MODFIFY or REMOVE it</t>
+  </si>
+  <si>
+    <t>hla</t>
+  </si>
+  <si>
+    <t>all of .csv file</t>
+  </si>
+  <si>
+    <t>reference table to prep data for hla-graph-database</t>
+  </si>
+  <si>
+    <t>aurau_test</t>
+  </si>
+  <si>
+    <t>test data tables for graph database with aurau, it will be removed aftre testing is done</t>
   </si>
 </sst>
 </file>
@@ -501,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D58D4F-E4E0-7B4B-B6D6-376651DC16AF}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,6 +562,9 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -558,6 +579,9 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -572,6 +596,9 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -724,6 +751,25 @@
       </c>
       <c r="E13" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>